<commit_message>
bao cao ca nhan - Vu
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Vu.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Vu.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Project</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>Chụp hình usecase minh chứng cho các chức năng trên</t>
+  </si>
+  <si>
+    <t>1 phần SDD</t>
+  </si>
+  <si>
+    <t>chưa hoàn thành</t>
+  </si>
+  <si>
+    <t>viết các chức năng SDD như SRS</t>
   </si>
 </sst>
 </file>
@@ -309,9 +318,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -329,6 +335,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,89 +668,109 @@
         <v>13</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>41173</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>3</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>41173</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0.5</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>0.5</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8">
+        <v>40918</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Vu sua bao cao
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Vu.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Vu.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Project</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>viết các chức năng SDD như SRS</t>
+  </si>
+  <si>
+    <t>24/9/2012</t>
+  </si>
+  <si>
+    <t>chỉnh sửa hoàn thiện SRS cá nhân</t>
+  </si>
+  <si>
+    <t>1phaanf SRS</t>
   </si>
 </sst>
 </file>
@@ -640,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -752,25 +761,47 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="8">
-        <v>40918</v>
+    <row r="6" spans="1:8" ht="40.5" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8">
+        <v>40918</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6">
+        <v>4</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>